<commit_message>
Update system.tex for SARP v2.0 compliance and revise experiment details
- Changed package settings comment to reflect SARP v2.0 compliance.
- Consolidated and organized package imports for circuit diagrams, code listings, and plots.
- Revised the experiment purpose to specify the use of a Sallen-Key low-pass filter.
- Updated the theoretical calculations section to clarify the derivation of transfer functions and parameters.
- Enhanced the experimental methods section with detailed equipment specifications and measurement procedures.
- Streamlined the results presentation, focusing on resonance peak measurements and their implications.
- Added MATLAB simulation results to validate theoretical and experimental findings.
- Updated the reference section for clarity and completeness.

Also, updated the associated Excel file with relevant data changes.
</commit_message>
<xml_diff>
--- a/Experiment/4/測定.xlsx
+++ b/Experiment/4/測定.xlsx
@@ -1,21 +1,34 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29426"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kaito\TeX-Folder\Experiment\4\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:9_{B7069CA2-FFD5-432B-9724-90FFF1ACB6A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B561B73-9625-4164-8129-DA3E6589234C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="29020" windowHeight="17500" xr2:uid="{29F7D881-C340-4110-805F-4D4332B7E1F0}"/>
   </bookViews>
   <sheets>
     <sheet name="2" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
@@ -69,9 +82,9 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="3">
-    <numFmt numFmtId="182" formatCode="0.000000000"/>
-    <numFmt numFmtId="187" formatCode="0.00000000000"/>
-    <numFmt numFmtId="188" formatCode="0.000000000000"/>
+    <numFmt numFmtId="176" formatCode="0.000000000"/>
+    <numFmt numFmtId="177" formatCode="0.00000000000"/>
+    <numFmt numFmtId="178" formatCode="0.000000000000"/>
   </numFmts>
   <fonts count="19" x14ac:knownFonts="1">
     <font>
@@ -669,19 +682,19 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="182" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
+    <xf numFmtId="176" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="182" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="187" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="188" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1">
+    <xf numFmtId="176" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="0" fillId="33" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1">
       <alignment vertical="center"/>
     </xf>
   </cellXfs>
@@ -975,7 +988,6 @@
           </c:extLst>
         </c:ser>
         <c:dLbls>
-          <c:dLblPos val="t"/>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
           <c:showCatName val="0"/>
@@ -3052,10 +3064,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{65A16A41-541F-4EBB-BC3F-AABF2E4720F8}">
-  <dimension ref="A1:M131"/>
+  <dimension ref="A1:M28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B2" zoomScale="81" zoomScaleNormal="209" workbookViewId="0">
-      <selection activeCell="J9" activeCellId="1" sqref="I9 J9"/>
+    <sheetView tabSelected="1" zoomScale="81" zoomScaleNormal="209" workbookViewId="0">
+      <selection activeCell="A30" sqref="A30"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="18" x14ac:dyDescent="0.55000000000000004"/>
@@ -3225,7 +3237,7 @@
         <v>1.0246913580246912</v>
       </c>
       <c r="F5">
-        <f t="shared" ref="F5:F31" si="2">20*LOG10(E5)</f>
+        <f t="shared" ref="F5:F25" si="2">20*LOG10(E5)</f>
         <v>0.21186146994848215</v>
       </c>
       <c r="G5" s="1">
@@ -3943,643 +3955,13 @@
       </c>
     </row>
     <row r="26" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="B26">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
       <c r="G26" s="1"/>
     </row>
     <row r="27" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="B27">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
       <c r="G27" s="1"/>
     </row>
     <row r="28" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="B28">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
       <c r="G28" s="1"/>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="B29">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="B30">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="B31">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.55000000000000004">
-      <c r="B32">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="B33">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="B34">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="B35">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="B36">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="B37">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="B38">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="B39">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="B40">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="B41">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="42" spans="2:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="B42">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="43" spans="2:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="B43">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="44" spans="2:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="B44">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="45" spans="2:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="B45">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="46" spans="2:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="B46">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="47" spans="2:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="B47">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="48" spans="2:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="B48">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="49" spans="2:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="B49">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="50" spans="2:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="B50">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="51" spans="2:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="B51">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="52" spans="2:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="B52">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="53" spans="2:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="B53">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="54" spans="2:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="B54">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="55" spans="2:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="B55">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="56" spans="2:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="B56">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="57" spans="2:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="B57">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="58" spans="2:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="B58">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="59" spans="2:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="B59">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="60" spans="2:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="B60">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="61" spans="2:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="B61">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="62" spans="2:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="B62">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="63" spans="2:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="B63">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="64" spans="2:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="B64">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="65" spans="2:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="B65">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="66" spans="2:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="B66">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="67" spans="2:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="B67">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="68" spans="2:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="B68">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="69" spans="2:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="B69">
-        <f t="shared" ref="B69:B131" si="5">A69*2*PI()</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="70" spans="2:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="B70">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="71" spans="2:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="B71">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="72" spans="2:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="B72">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="73" spans="2:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="B73">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="74" spans="2:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="B74">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="75" spans="2:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="B75">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="76" spans="2:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="B76">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="77" spans="2:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="B77">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="78" spans="2:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="B78">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="79" spans="2:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="B79">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="80" spans="2:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="B80">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="81" spans="2:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="B81">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="82" spans="2:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="B82">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="83" spans="2:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="B83">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="84" spans="2:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="B84">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="85" spans="2:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="B85">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="86" spans="2:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="B86">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="87" spans="2:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="B87">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="88" spans="2:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="B88">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="89" spans="2:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="B89">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="90" spans="2:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="B90">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="91" spans="2:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="B91">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="92" spans="2:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="B92">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="93" spans="2:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="B93">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="94" spans="2:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="B94">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="95" spans="2:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="B95">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="96" spans="2:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="B96">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="97" spans="2:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="B97">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="98" spans="2:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="B98">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="99" spans="2:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="B99">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="100" spans="2:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="B100">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="101" spans="2:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="B101">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="102" spans="2:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="B102">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="103" spans="2:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="B103">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="104" spans="2:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="B104">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="105" spans="2:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="B105">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="106" spans="2:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="B106">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="107" spans="2:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="B107">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="108" spans="2:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="B108">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="109" spans="2:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="B109">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="110" spans="2:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="B110">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="111" spans="2:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="B111">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="112" spans="2:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="B112">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="113" spans="2:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="B113">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="114" spans="2:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="B114">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="115" spans="2:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="B115">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="116" spans="2:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="B116">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="117" spans="2:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="B117">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="118" spans="2:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="B118">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="119" spans="2:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="B119">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="120" spans="2:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="B120">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="121" spans="2:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="B121">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="122" spans="2:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="B122">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="123" spans="2:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="B123">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="124" spans="2:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="B124">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="125" spans="2:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="B125">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="126" spans="2:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="B126">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="127" spans="2:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="B127">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="128" spans="2:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="B128">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="129" spans="2:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="B129">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="130" spans="2:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="B130">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="131" spans="2:2" x14ac:dyDescent="0.55000000000000004">
-      <c r="B131">
-        <f t="shared" si="5"/>
-        <v>0</v>
-      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="18"/>

</xml_diff>